<commit_message>
integrated lists and word trigger lists
</commit_message>
<xml_diff>
--- a/ExcelHO/Finanzen 2017.xlsx
+++ b/ExcelHO/Finanzen 2017.xlsx
@@ -1358,19 +1358,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="168" fontId="8" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="168" fontId="8" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="168" fontId="8" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="168" fontId="8" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -31222,7 +31222,7 @@
       <c r="Z15" s="82"/>
     </row>
     <row r="16" spans="1:26">
-      <c r="A16" s="100">
+      <c r="A16" s="99">
         <v>42614</v>
       </c>
       <c r="B16" s="83" t="s">
@@ -31604,7 +31604,7 @@
       <c r="L27" s="44"/>
     </row>
     <row r="28" spans="1:26">
-      <c r="A28" s="100">
+      <c r="A28" s="99">
         <v>42618</v>
       </c>
       <c r="B28" s="83" t="s">
@@ -32257,7 +32257,7 @@
       <c r="Z53" s="55"/>
     </row>
     <row r="54" spans="1:26">
-      <c r="A54" s="101">
+      <c r="A54" s="102">
         <v>42635</v>
       </c>
       <c r="B54" s="41"/>
@@ -32381,7 +32381,7 @@
       <c r="L59" s="44"/>
     </row>
     <row r="60" spans="1:26">
-      <c r="A60" s="100">
+      <c r="A60" s="99">
         <v>42640</v>
       </c>
       <c r="B60" t="s">
@@ -32498,7 +32498,7 @@
       <c r="L63" s="44"/>
     </row>
     <row r="64" spans="1:26">
-      <c r="A64" s="100">
+      <c r="A64" s="99">
         <v>42642</v>
       </c>
       <c r="C64" s="52"/>
@@ -32933,7 +32933,7 @@
       <c r="Z15" s="82"/>
     </row>
     <row r="16" spans="1:26">
-      <c r="A16" s="100">
+      <c r="A16" s="99">
         <v>42644</v>
       </c>
       <c r="B16" s="41" t="s">
@@ -33130,7 +33130,7 @@
       <c r="L22" s="44"/>
     </row>
     <row r="23" spans="1:26">
-      <c r="A23" s="100">
+      <c r="A23" s="99">
         <v>42618</v>
       </c>
       <c r="B23" s="54" t="s">
@@ -33282,7 +33282,7 @@
       <c r="L28" s="44"/>
     </row>
     <row r="29" spans="1:26">
-      <c r="A29" s="102">
+      <c r="A29" s="103">
         <v>42620</v>
       </c>
       <c r="B29" s="54" t="s">
@@ -33472,7 +33472,7 @@
       <c r="L35" s="44"/>
     </row>
     <row r="36" spans="1:26">
-      <c r="A36" s="102">
+      <c r="A36" s="103">
         <v>42624</v>
       </c>
       <c r="B36" s="54" t="s">
@@ -33558,7 +33558,7 @@
       <c r="L38" s="44"/>
     </row>
     <row r="39" spans="1:26">
-      <c r="A39" s="100">
+      <c r="A39" s="99">
         <v>42626</v>
       </c>
       <c r="B39" s="54" t="s">
@@ -33966,7 +33966,7 @@
       <c r="L53" s="44"/>
     </row>
     <row r="54" spans="1:26">
-      <c r="A54" s="100">
+      <c r="A54" s="99">
         <v>42632</v>
       </c>
       <c r="B54" s="54" t="s">
@@ -34032,7 +34032,7 @@
       <c r="Z55" s="55"/>
     </row>
     <row r="56" spans="1:26">
-      <c r="A56" s="101">
+      <c r="A56" s="102">
         <v>42633</v>
       </c>
       <c r="B56" s="54" t="s">
@@ -34088,7 +34088,7 @@
       <c r="L58" s="44"/>
     </row>
     <row r="59" spans="1:26">
-      <c r="A59" s="102">
+      <c r="A59" s="103">
         <v>42634</v>
       </c>
       <c r="B59" s="41" t="s">
@@ -34340,7 +34340,7 @@
       <c r="L68" s="44"/>
     </row>
     <row r="69" spans="1:26">
-      <c r="A69" s="100">
+      <c r="A69" s="99">
         <v>42640</v>
       </c>
       <c r="B69" s="70" t="s">
@@ -34523,7 +34523,7 @@
       <c r="L75" s="44"/>
     </row>
     <row r="76" spans="1:26">
-      <c r="A76" s="100">
+      <c r="A76" s="99">
         <v>42642</v>
       </c>
       <c r="B76" s="70" t="s">
@@ -34716,6 +34716,18 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A43:A45"/>
     <mergeCell ref="A56:A58"/>
     <mergeCell ref="A78:A81"/>
     <mergeCell ref="A82:A83"/>
@@ -34723,18 +34735,6 @@
     <mergeCell ref="A63:A65"/>
     <mergeCell ref="A76:A77"/>
     <mergeCell ref="A69:A72"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A43:A45"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A34:A35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -34981,7 +34981,7 @@
       <c r="Z15" s="82"/>
     </row>
     <row r="16" spans="1:26">
-      <c r="A16" s="100">
+      <c r="A16" s="99">
         <v>42675</v>
       </c>
       <c r="B16" s="41" t="s">
@@ -35168,7 +35168,7 @@
       <c r="L22" s="44"/>
     </row>
     <row r="23" spans="1:26">
-      <c r="A23" s="100">
+      <c r="A23" s="99">
         <v>42677</v>
       </c>
       <c r="B23" s="41" t="s">
@@ -35392,7 +35392,7 @@
       <c r="L30" s="44"/>
     </row>
     <row r="31" spans="1:26">
-      <c r="A31" s="102">
+      <c r="A31" s="103">
         <v>42681</v>
       </c>
       <c r="B31" s="41" t="s">
@@ -35496,7 +35496,7 @@
       <c r="L34" s="44"/>
     </row>
     <row r="35" spans="1:26">
-      <c r="A35" s="102">
+      <c r="A35" s="103">
         <v>42683</v>
       </c>
       <c r="B35" s="41" t="s">
@@ -35668,7 +35668,7 @@
       <c r="L40" s="44"/>
     </row>
     <row r="41" spans="1:26">
-      <c r="A41" s="102">
+      <c r="A41" s="103">
         <v>42685</v>
       </c>
       <c r="B41" s="41" t="s">
@@ -36282,7 +36282,7 @@
       <c r="L64" s="44"/>
     </row>
     <row r="65" spans="1:26">
-      <c r="A65" s="102">
+      <c r="A65" s="103">
         <v>42695</v>
       </c>
       <c r="B65" s="41" t="s">
@@ -36380,7 +36380,7 @@
       <c r="Z67" s="55"/>
     </row>
     <row r="68" spans="1:26">
-      <c r="A68" s="101">
+      <c r="A68" s="102">
         <v>42696</v>
       </c>
       <c r="B68" s="41" t="s">
@@ -36472,7 +36472,7 @@
       <c r="L72" s="44"/>
     </row>
     <row r="73" spans="1:26">
-      <c r="A73" s="100">
+      <c r="A73" s="99">
         <v>42697</v>
       </c>
       <c r="B73" s="41" t="s">
@@ -36632,7 +36632,7 @@
       <c r="L78" s="44"/>
     </row>
     <row r="79" spans="1:26">
-      <c r="A79" s="100">
+      <c r="A79" s="99">
         <v>42699</v>
       </c>
       <c r="B79" s="41" t="s">
@@ -36953,13 +36953,11 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A35:A38"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A88:A89"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="A68:A72"/>
     <mergeCell ref="A59:A62"/>
     <mergeCell ref="A65:A67"/>
     <mergeCell ref="A39:A40"/>
@@ -36970,11 +36968,13 @@
     <mergeCell ref="A49:A51"/>
     <mergeCell ref="A46:A48"/>
     <mergeCell ref="A52:A54"/>
-    <mergeCell ref="A88:A89"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="A68:A72"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A33:A34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -37220,7 +37220,7 @@
       <c r="Z15" s="82"/>
     </row>
     <row r="16" spans="1:26">
-      <c r="A16" s="100">
+      <c r="A16" s="99">
         <v>42644</v>
       </c>
       <c r="B16" s="41" t="s">
@@ -37500,7 +37500,7 @@
       <c r="L26" s="44"/>
     </row>
     <row r="27" spans="1:26">
-      <c r="A27" s="100">
+      <c r="A27" s="99">
         <v>42618</v>
       </c>
       <c r="B27" s="41" t="s">
@@ -37642,7 +37642,7 @@
       <c r="L32" s="44"/>
     </row>
     <row r="33" spans="1:26">
-      <c r="A33" s="102">
+      <c r="A33" s="103">
         <v>42620</v>
       </c>
       <c r="B33" s="41" t="s">
@@ -37874,7 +37874,7 @@
       <c r="L41" s="44"/>
     </row>
     <row r="42" spans="1:26">
-      <c r="A42" s="102">
+      <c r="A42" s="103">
         <v>42624</v>
       </c>
       <c r="B42" s="41" t="s">
@@ -38010,7 +38010,7 @@
       <c r="L47" s="44"/>
     </row>
     <row r="48" spans="1:26">
-      <c r="A48" s="100">
+      <c r="A48" s="99">
         <v>42626</v>
       </c>
       <c r="B48" s="41" t="s">
@@ -38488,7 +38488,7 @@
       <c r="L66" s="44"/>
     </row>
     <row r="67" spans="1:26">
-      <c r="A67" s="100">
+      <c r="A67" s="99">
         <v>42632</v>
       </c>
       <c r="B67" s="41" t="s">
@@ -38550,7 +38550,7 @@
       <c r="Z68" s="55"/>
     </row>
     <row r="69" spans="1:26">
-      <c r="A69" s="101">
+      <c r="A69" s="102">
         <v>42633</v>
       </c>
       <c r="B69" s="41" t="s">
@@ -38606,7 +38606,7 @@
       <c r="L71" s="44"/>
     </row>
     <row r="72" spans="1:26">
-      <c r="A72" s="102">
+      <c r="A72" s="103">
         <v>42634</v>
       </c>
       <c r="B72" s="41" t="s">
@@ -38924,7 +38924,7 @@
       <c r="L85" s="44"/>
     </row>
     <row r="86" spans="1:26">
-      <c r="A86" s="100">
+      <c r="A86" s="99">
         <v>42640</v>
       </c>
       <c r="C86" s="52"/>
@@ -39094,7 +39094,7 @@
       <c r="L93" s="44"/>
     </row>
     <row r="94" spans="1:26">
-      <c r="A94" s="100">
+      <c r="A94" s="99">
         <v>42642</v>
       </c>
       <c r="C94" s="52"/>
@@ -39290,6 +39290,18 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="A64:A66"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A16:A19"/>
     <mergeCell ref="A69:A71"/>
     <mergeCell ref="A86:A89"/>
     <mergeCell ref="A94:A95"/>
@@ -39297,18 +39309,6 @@
     <mergeCell ref="A100:A101"/>
     <mergeCell ref="A80:A82"/>
     <mergeCell ref="A72:A73"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="A60:A63"/>
-    <mergeCell ref="A64:A66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -43104,8 +43104,8 @@
   <dimension ref="A1:Z101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="14" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
+      <pane ySplit="14" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
@@ -44771,22 +44771,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A82:A85"/>
-    <mergeCell ref="A86:A89"/>
-    <mergeCell ref="A92:A93"/>
-    <mergeCell ref="A95:A96"/>
-    <mergeCell ref="A77:A80"/>
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="A64:A68"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="A71:A73"/>
-    <mergeCell ref="A53:A55"/>
     <mergeCell ref="A47:A49"/>
     <mergeCell ref="A33:A35"/>
     <mergeCell ref="A29:A31"/>
     <mergeCell ref="A22:A24"/>
     <mergeCell ref="A19:A21"/>
     <mergeCell ref="A37:A40"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="A64:A68"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="A71:A73"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="A82:A85"/>
+    <mergeCell ref="A86:A89"/>
+    <mergeCell ref="A92:A93"/>
+    <mergeCell ref="A95:A96"/>
+    <mergeCell ref="A77:A80"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -45287,7 +45287,7 @@
       <c r="L29" s="44"/>
     </row>
     <row r="30" spans="1:26">
-      <c r="A30" s="99">
+      <c r="A30" s="101">
         <v>42556</v>
       </c>
       <c r="B30" t="s">
@@ -45385,7 +45385,7 @@
       <c r="L34" s="44"/>
     </row>
     <row r="35" spans="1:21">
-      <c r="A35" s="102">
+      <c r="A35" s="103">
         <v>42558</v>
       </c>
       <c r="B35" t="s">
@@ -45514,7 +45514,7 @@
       <c r="L41" s="44"/>
     </row>
     <row r="42" spans="1:21">
-      <c r="A42" s="102">
+      <c r="A42" s="103">
         <v>42560</v>
       </c>
       <c r="C42" s="44"/>
@@ -45590,7 +45590,7 @@
       <c r="L45" s="44"/>
     </row>
     <row r="46" spans="1:21">
-      <c r="A46" s="102">
+      <c r="A46" s="103">
         <v>42562</v>
       </c>
       <c r="B46" t="s">
@@ -45723,7 +45723,7 @@
       <c r="L51" s="44"/>
     </row>
     <row r="52" spans="1:21">
-      <c r="A52" s="100">
+      <c r="A52" s="99">
         <v>42564</v>
       </c>
       <c r="B52" s="41"/>
@@ -45821,7 +45821,7 @@
       <c r="L57" s="44"/>
     </row>
     <row r="58" spans="1:21">
-      <c r="A58" s="100">
+      <c r="A58" s="99">
         <v>42566</v>
       </c>
       <c r="B58" t="s">
@@ -45939,7 +45939,7 @@
       <c r="L63" s="44"/>
     </row>
     <row r="64" spans="1:21">
-      <c r="A64" s="100">
+      <c r="A64" s="99">
         <v>42570</v>
       </c>
       <c r="B64" t="s">
@@ -46028,7 +46028,7 @@
       <c r="L67" s="44"/>
     </row>
     <row r="68" spans="1:20">
-      <c r="A68" s="102">
+      <c r="A68" s="103">
         <v>42572</v>
       </c>
       <c r="B68" t="s">
@@ -46093,7 +46093,7 @@
       <c r="O70" s="55"/>
     </row>
     <row r="71" spans="1:20">
-      <c r="A71" s="101">
+      <c r="A71" s="102">
         <v>42573</v>
       </c>
       <c r="B71" s="45" t="s">
@@ -46127,7 +46127,7 @@
       <c r="L72" s="44"/>
     </row>
     <row r="73" spans="1:20">
-      <c r="A73" s="100">
+      <c r="A73" s="99">
         <v>42574</v>
       </c>
       <c r="C73" s="44"/>
@@ -46177,7 +46177,7 @@
       <c r="O75" s="55"/>
     </row>
     <row r="76" spans="1:20">
-      <c r="A76" s="103">
+      <c r="A76" s="100">
         <v>42575</v>
       </c>
       <c r="C76" s="44"/>
@@ -46205,7 +46205,7 @@
       <c r="L77" s="44"/>
     </row>
     <row r="78" spans="1:20">
-      <c r="A78" s="100">
+      <c r="A78" s="99">
         <v>42576</v>
       </c>
       <c r="C78" s="44"/>
@@ -46303,7 +46303,7 @@
       <c r="L82" s="44"/>
     </row>
     <row r="83" spans="1:15">
-      <c r="A83" s="100">
+      <c r="A83" s="99">
         <v>42578</v>
       </c>
       <c r="C83" s="44"/>
@@ -46381,7 +46381,7 @@
       <c r="L87" s="44"/>
     </row>
     <row r="88" spans="1:15">
-      <c r="A88" s="100">
+      <c r="A88" s="99">
         <v>42580</v>
       </c>
       <c r="C88" s="44"/>
@@ -46570,12 +46570,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A96:A100"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="A73:A75"/>
-    <mergeCell ref="A76:A77"/>
-    <mergeCell ref="A78:A80"/>
-    <mergeCell ref="A81:A82"/>
     <mergeCell ref="A33:A34"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="A28:A29"/>
@@ -46591,6 +46585,12 @@
     <mergeCell ref="A46:A49"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A96:A100"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="A73:A75"/>
+    <mergeCell ref="A76:A77"/>
+    <mergeCell ref="A78:A80"/>
+    <mergeCell ref="A81:A82"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -46839,7 +46839,7 @@
       <c r="F18" s="47"/>
     </row>
     <row r="19" spans="1:26">
-      <c r="A19" s="100">
+      <c r="A19" s="99">
         <v>42583</v>
       </c>
       <c r="B19" s="54" t="s">
@@ -46963,7 +46963,7 @@
       <c r="L22" s="44"/>
     </row>
     <row r="23" spans="1:26">
-      <c r="A23" s="100">
+      <c r="A23" s="99">
         <v>42585</v>
       </c>
       <c r="B23" s="54" t="s">
@@ -47083,7 +47083,7 @@
       <c r="L27" s="44"/>
     </row>
     <row r="28" spans="1:26">
-      <c r="A28" s="100">
+      <c r="A28" s="99">
         <v>42587</v>
       </c>
       <c r="B28" s="54" t="s">
@@ -47313,7 +47313,7 @@
       <c r="L37" s="44"/>
     </row>
     <row r="38" spans="1:26">
-      <c r="A38" s="102">
+      <c r="A38" s="103">
         <v>42589</v>
       </c>
       <c r="B38" s="54" t="s">
@@ -47416,7 +47416,7 @@
       <c r="L41" s="44"/>
     </row>
     <row r="42" spans="1:26">
-      <c r="A42" s="102">
+      <c r="A42" s="103">
         <v>42591</v>
       </c>
       <c r="B42" s="54" t="s">
@@ -47626,7 +47626,7 @@
       <c r="Z49" s="55"/>
     </row>
     <row r="50" spans="1:26">
-      <c r="A50" s="101">
+      <c r="A50" s="102">
         <v>42594</v>
       </c>
       <c r="B50" s="54" t="s">
@@ -47962,7 +47962,7 @@
       <c r="L64" s="44"/>
     </row>
     <row r="65" spans="1:26">
-      <c r="A65" s="100">
+      <c r="A65" s="99">
         <v>42570</v>
       </c>
       <c r="B65" s="54" t="s">
@@ -48110,7 +48110,7 @@
       <c r="Z69" s="55"/>
     </row>
     <row r="70" spans="1:26">
-      <c r="A70" s="101">
+      <c r="A70" s="102">
         <v>42573</v>
       </c>
       <c r="B70" s="54" t="s">
@@ -48148,7 +48148,7 @@
       <c r="L71" s="44"/>
     </row>
     <row r="72" spans="1:26">
-      <c r="A72" s="100">
+      <c r="A72" s="99">
         <v>42574</v>
       </c>
       <c r="B72" s="54" t="s">
@@ -48388,7 +48388,7 @@
       <c r="L80" s="44"/>
     </row>
     <row r="81" spans="1:26">
-      <c r="A81" s="100">
+      <c r="A81" s="99">
         <v>42580</v>
       </c>
       <c r="B81" s="70" t="s">
@@ -48517,7 +48517,7 @@
       </c>
     </row>
     <row r="87" spans="1:26">
-      <c r="A87" s="100">
+      <c r="A87" s="99">
         <v>42582</v>
       </c>
       <c r="B87" s="54" t="s">
@@ -48615,17 +48615,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="A83:A86"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A87:A88"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="A75:A76"/>
-    <mergeCell ref="A72:A74"/>
-    <mergeCell ref="A70:A71"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="A19:A21"/>
     <mergeCell ref="A42:A44"/>
@@ -48636,6 +48625,17 @@
     <mergeCell ref="A31:A37"/>
     <mergeCell ref="A25:A27"/>
     <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A87:A88"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="A75:A76"/>
+    <mergeCell ref="A72:A74"/>
+    <mergeCell ref="A70:A71"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="A83:A86"/>
+    <mergeCell ref="A81:A82"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>